<commit_message>
2013 in progress, includes 2014
</commit_message>
<xml_diff>
--- a/CLEAN DATA/The Boardroom Group/progress.xlsx
+++ b/CLEAN DATA/The Boardroom Group/progress.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9691" uniqueCount="4198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9783" uniqueCount="4239">
   <si>
     <t>Homelessness Secretariat</t>
   </si>
@@ -13113,12 +13113,135 @@
   <si>
     <t>4:39|5:0|12:150</t>
   </si>
+  <si>
+    <t>Out of the Rain</t>
+  </si>
+  <si>
+    <t>Dawn to Dawn</t>
+  </si>
+  <si>
+    <t>Pacific Community Resources Society Youth Services</t>
+  </si>
+  <si>
+    <t>Lookout Emergency Aid Society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seasons House </t>
+  </si>
+  <si>
+    <t>Centre of Hope</t>
+  </si>
+  <si>
+    <t>Servants Anonymous Society of Calgary</t>
+  </si>
+  <si>
+    <t>Calgary John Howard Society: Raido House</t>
+  </si>
+  <si>
+    <t>Homeward Trust Edmonton</t>
+  </si>
+  <si>
+    <t>Rainbow Youth Centre</t>
+  </si>
+  <si>
+    <t>Macdonald Youth Services</t>
+  </si>
+  <si>
+    <t>Stratford/Perth Shelterlink</t>
+  </si>
+  <si>
+    <t>The Hope Centre</t>
+  </si>
+  <si>
+    <t>YWCA Niagara Region</t>
+  </si>
+  <si>
+    <t>Community Care - St. Cath &amp; Thorold</t>
+  </si>
+  <si>
+    <t>Wesley Urban Ministries Inc.</t>
+  </si>
+  <si>
+    <t>360 kids</t>
+  </si>
+  <si>
+    <t>Houselink Community</t>
+  </si>
+  <si>
+    <t>St. Christopher House</t>
+  </si>
+  <si>
+    <t>Sherbourne Health Centre</t>
+  </si>
+  <si>
+    <t>Grimsby Affordable Housing Partnership</t>
+  </si>
+  <si>
+    <t>Port Cares</t>
+  </si>
+  <si>
+    <t>Sudbury Action Centre for Youth</t>
+  </si>
+  <si>
+    <t>Couchiching Jubilee House</t>
+  </si>
+  <si>
+    <t>Operation Come Home</t>
+  </si>
+  <si>
+    <t>Cornerstone Landing ER</t>
+  </si>
+  <si>
+    <t>Youth Opportunities Limited</t>
+  </si>
+  <si>
+    <t>Groupe Communautaire L'Itinéraire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spectre de rue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maison Le Baluchon </t>
+  </si>
+  <si>
+    <t>RAP Jeunesse des Laurentides</t>
+  </si>
+  <si>
+    <t>YWCA Halifax</t>
+  </si>
+  <si>
+    <t>Bryony House</t>
+  </si>
+  <si>
+    <t>SHYFT</t>
+  </si>
+  <si>
+    <t>Pictou County Roots for Youth</t>
+  </si>
+  <si>
+    <t>Saint John Human Development Council - Safe Harbour</t>
+  </si>
+  <si>
+    <t>Moncton Youth Residences</t>
+  </si>
+  <si>
+    <t>Labrador Friendship Centre</t>
+  </si>
+  <si>
+    <t>Community Youth Network / Humber Community YMCA</t>
+  </si>
+  <si>
+    <t>Choices for Youth</t>
+  </si>
+  <si>
+    <t>Newfoundland &amp; Labrador Housing &amp; Homelessness Network</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13167,12 +13290,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -13624,11 +13741,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2660"/>
+  <dimension ref="A1:I2687"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2611" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2640" sqref="C2640"/>
+      <pane ySplit="1" topLeftCell="A2642" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2687" sqref="A2687"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -77151,104 +77268,653 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2641" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2641" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2641" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2642" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2641" s="4" t="s">
+        <v>4198</v>
+      </c>
+      <c r="D2641" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2641" s="4">
+        <v>2287.15</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2642" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2643" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2642" s="4" t="s">
+        <v>4199</v>
+      </c>
+      <c r="D2642" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2642" s="4">
+        <v>1955</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2643" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2644" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2643" s="4" t="s">
+        <v>4200</v>
+      </c>
+      <c r="D2643" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2643" s="4">
+        <v>6389.5</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2644" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2645" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2644" s="4" t="s">
+        <v>4201</v>
+      </c>
+      <c r="D2644" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2644" s="4">
+        <v>8202.5</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2645" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2646" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2645" s="4" t="s">
+        <v>4202</v>
+      </c>
+      <c r="D2645" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2645" s="4">
+        <v>3860</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2646" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2647" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2646" s="4" t="s">
+        <v>4203</v>
+      </c>
+      <c r="D2646" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2646" s="4">
+        <v>6090</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2647" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2648" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2647" s="4" t="s">
+        <v>4204</v>
+      </c>
+      <c r="D2647" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2647" s="4">
+        <v>12260.67</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2648" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2649" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2648" s="4" t="s">
+        <v>4205</v>
+      </c>
+      <c r="D2648" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2648" s="4">
+        <v>4475.6900000000005</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2649" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2650" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2649" s="4" t="s">
+        <v>4206</v>
+      </c>
+      <c r="D2649" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2649" s="4">
+        <v>17726.510000000002</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2650" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2651" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2650" s="4" t="s">
+        <v>4207</v>
+      </c>
+      <c r="D2650" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2650" s="4">
+        <v>5960</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2651" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2652" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2651" s="4" t="s">
+        <v>4208</v>
+      </c>
+      <c r="D2651" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2651" s="4">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2652" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2653" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2652" s="4" t="s">
+        <v>4209</v>
+      </c>
+      <c r="D2652" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2652" s="4">
+        <v>4310</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2653" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2654" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2653" s="4" t="s">
+        <v>4210</v>
+      </c>
+      <c r="D2653" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2653" s="4">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2654" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2655" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2654" s="4" t="s">
+        <v>1937</v>
+      </c>
+      <c r="D2654" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2654" s="4">
+        <v>3134.75</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2655" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2656" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2655" s="4" t="s">
+        <v>4211</v>
+      </c>
+      <c r="D2655" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2655" s="4">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2656" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2657" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2656" s="4" t="s">
+        <v>4212</v>
+      </c>
+      <c r="D2656" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2656" s="4">
+        <v>19855.14</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2657" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2658" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2657" s="4" t="s">
+        <v>4213</v>
+      </c>
+      <c r="D2657" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2657" s="4">
+        <v>13113</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2658" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2659" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2658" s="4" t="s">
+        <v>4214</v>
+      </c>
+      <c r="D2658" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2658" s="4">
+        <v>20685.599999999999</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2659" s="4">
-        <v>2011</v>
-      </c>
-    </row>
-    <row r="2660" spans="1:1" x14ac:dyDescent="0.2">
+        <v>2014</v>
+      </c>
+      <c r="C2659" s="4" t="s">
+        <v>4215</v>
+      </c>
+      <c r="D2659" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2659" s="4">
+        <v>11094.53</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2660" s="4">
-        <v>2011</v>
+        <v>2014</v>
+      </c>
+      <c r="C2660" s="4" t="s">
+        <v>4216</v>
+      </c>
+      <c r="D2660" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2660" s="4">
+        <v>9986.7800000000007</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2661" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2661" s="4" t="s">
+        <v>4217</v>
+      </c>
+      <c r="D2661" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2661" s="4">
+        <v>15235.119999999999</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2662" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2662" s="4" t="s">
+        <v>2912</v>
+      </c>
+      <c r="D2662" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2662" s="4">
+        <v>11580</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2663" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2663" s="4" t="s">
+        <v>4218</v>
+      </c>
+      <c r="D2663" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2663" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2664" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2664" s="4" t="s">
+        <v>4219</v>
+      </c>
+      <c r="D2664" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2664" s="4">
+        <v>4090.57</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2665" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2665" s="4" t="s">
+        <v>4220</v>
+      </c>
+      <c r="D2665" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2665" s="4">
+        <v>3060</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2666" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2666" s="4" t="s">
+        <v>4221</v>
+      </c>
+      <c r="D2666" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2666" s="4">
+        <v>4600.6000000000004</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2667" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2667" s="4" t="s">
+        <v>4222</v>
+      </c>
+      <c r="D2667" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2667" s="4">
+        <v>10356</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2668" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2668" s="4" t="s">
+        <v>4223</v>
+      </c>
+      <c r="D2668" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2668" s="4">
+        <v>4382</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2669" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2669" s="4" t="s">
+        <v>4224</v>
+      </c>
+      <c r="D2669" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2669" s="4">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2670" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2670" s="4" t="s">
+        <v>4225</v>
+      </c>
+      <c r="D2670" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2670" s="4">
+        <v>7741</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2671" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2671" s="4" t="s">
+        <v>4226</v>
+      </c>
+      <c r="D2671" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2671" s="4">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2672" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2672" s="4" t="s">
+        <v>4227</v>
+      </c>
+      <c r="D2672" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2672" s="4">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2673" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2673" s="4" t="s">
+        <v>4228</v>
+      </c>
+      <c r="D2673" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2673" s="4">
+        <v>2267</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2674" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2674" s="4" t="s">
+        <v>4229</v>
+      </c>
+      <c r="D2674" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2674" s="4">
+        <v>3199.05</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2675" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2675" s="4" t="s">
+        <v>4230</v>
+      </c>
+      <c r="D2675" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2675" s="4">
+        <v>4896.6499999999996</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2676" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2676" s="4" t="s">
+        <v>4231</v>
+      </c>
+      <c r="D2676" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2676" s="4">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2677" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2677" s="4" t="s">
+        <v>4232</v>
+      </c>
+      <c r="D2677" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2677" s="4">
+        <v>3765</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2678" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2678" s="4" t="s">
+        <v>4233</v>
+      </c>
+      <c r="D2678" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2678" s="4">
+        <v>1481</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2679" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2679" s="4" t="s">
+        <v>4234</v>
+      </c>
+      <c r="D2679" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2679" s="4">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2680" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2680" s="4" t="s">
+        <v>4235</v>
+      </c>
+      <c r="D2680" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2680" s="4">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2681" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2681" s="4" t="s">
+        <v>4236</v>
+      </c>
+      <c r="D2681" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2681" s="4">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2682" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2682" s="4" t="s">
+        <v>4237</v>
+      </c>
+      <c r="D2682" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2682" s="4">
+        <v>1697.5</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2683" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2683" s="4" t="s">
+        <v>4238</v>
+      </c>
+      <c r="D2683" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2683" s="4">
+        <v>2907.5</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2684" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2684" s="4" t="s">
+        <v>4172</v>
+      </c>
+      <c r="D2684" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2684" s="4">
+        <v>116000</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2685" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2685" s="4" t="s">
+        <v>3956</v>
+      </c>
+      <c r="D2685" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2685" s="4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2686" s="4">
+        <v>2014</v>
+      </c>
+      <c r="C2686" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2686" s="4" t="s">
+        <v>849</v>
+      </c>
+      <c r="H2686" s="4">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2687" s="4">
+        <v>2015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>